<commit_message>
Corrected VirSorter datasets used
</commit_message>
<xml_diff>
--- a/data/Viromes_data.xlsx
+++ b/data/Viromes_data.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="600" windowWidth="38400" windowHeight="17595"/>
+    <workbookView xWindow="0" yWindow="600" windowWidth="38370" windowHeight="17580"/>
   </bookViews>
   <sheets>
     <sheet name="Viromes_data" sheetId="1" r:id="rId1"/>
@@ -6667,7 +6667,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="73" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="75.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="16.140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="94" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="9.28515625" bestFit="1" customWidth="1"/>
@@ -6678,6 +6678,7 @@
     <col min="9" max="10" width="76.28515625" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="37.5703125" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="38.7109375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="9.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">

</xml_diff>